<commit_message>
Create basic tests and output
</commit_message>
<xml_diff>
--- a/test/spreadsheets/projects.xlsx
+++ b/test/spreadsheets/projects.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\In Development\Ambition for Ageing monitoring system\Manchester Imports Preparation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\ICT ENTERPRISE\Projects\In Development\Ambition for Ageing monitoring system\Manchester Imports Preparation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="19845" windowHeight="8310"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19845" windowHeight="4110"/>
   </bookViews>
   <sheets>
     <sheet name="Fields to Import" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
   <si>
     <t>Organisation Name</t>
   </si>
@@ -152,6 +152,21 @@
   </si>
   <si>
     <t>External Identifier</t>
+  </si>
+  <si>
+    <t>Project Start Date</t>
+  </si>
+  <si>
+    <t>Project End Date</t>
+  </si>
+  <si>
+    <t>Date field</t>
+  </si>
+  <si>
+    <t>If possible please provide dates in format yyyy-mm-dd</t>
+  </si>
+  <si>
+    <t>Approximate/estimated end dates accepted</t>
   </si>
 </sst>
 </file>
@@ -973,36 +988,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:V4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="59.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="33" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="59.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="59.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.85546875" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -1028,43 +1022,49 @@
         <v>6</v>
       </c>
       <c r="I1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -1090,43 +1090,49 @@
         <v>25</v>
       </c>
       <c r="I2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2" t="s">
         <v>24</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>19</v>
-      </c>
-      <c r="K2" t="s">
-        <v>27</v>
-      </c>
-      <c r="L2" t="s">
-        <v>28</v>
       </c>
       <c r="M2" t="s">
         <v>27</v>
       </c>
       <c r="N2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O2" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="P2" t="s">
         <v>29</v>
       </c>
       <c r="Q2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R2" t="s">
+        <v>29</v>
+      </c>
+      <c r="S2" t="s">
         <v>34</v>
       </c>
-      <c r="R2" t="s">
+      <c r="T2" t="s">
         <v>34</v>
       </c>
-      <c r="S2" t="s">
+      <c r="U2" t="s">
         <v>27</v>
       </c>
-      <c r="T2" t="s">
+      <c r="V2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:20" s="3" customFormat="1" ht="375" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" s="3" customFormat="1" ht="375" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
@@ -1144,34 +1150,43 @@
         <v>31</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
-      <c r="N3" s="1" t="s">
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="O3" s="1"/>
-      <c r="P3" s="2" t="s">
+      <c r="Q3" s="1"/>
+      <c r="R3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
       <c r="S3" s="1"/>
-      <c r="T3" s="1" t="s">
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="H4" t="s">
         <v>30</v>
       </c>
-      <c r="N4" t="s">
+      <c r="J4" t="s">
+        <v>42</v>
+      </c>
+      <c r="P4" t="s">
         <v>30</v>
       </c>
-      <c r="P4" t="s">
+      <c r="R4" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>